<commit_message>
melakukan perubahan pada excel
</commit_message>
<xml_diff>
--- a/Product Backlog+User Story.xlsx
+++ b/Product Backlog+User Story.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Music\sem4\3 agile\figma n laporan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\version control git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0013940F-ED6B-440D-8B00-F111FA827B48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5145200-554E-4AEE-A494-B6BEEB47CF8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2E39C133-9BD4-4088-A2A7-6E9E70B08AB9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2E39C133-9BD4-4088-A2A7-6E9E70B08AB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$7:$H$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$8:$H$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="112">
   <si>
     <t>ID</t>
   </si>
@@ -361,6 +361,15 @@
   </si>
   <si>
     <t>Dimulai 3/5/2023</t>
+  </si>
+  <si>
+    <t>Product Backlog dan User Story</t>
+  </si>
+  <si>
+    <t>ScreenShoot Trello board ada di paling bawah</t>
+  </si>
+  <si>
+    <t>Screenshot board trello</t>
   </si>
 </sst>
 </file>
@@ -446,7 +455,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -778,6 +787,116 @@
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -785,7 +904,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -838,15 +957,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -856,96 +966,125 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1018,6 +1157,161 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>367392</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>27214</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>832756</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>15555</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E69414D-9BF8-A6C0-F0A1-375F8B198DAF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="979713" y="31092321"/>
+          <a:ext cx="7772400" cy="4369841"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>354107</xdr:colOff>
+      <xdr:row>123</xdr:row>
+      <xdr:rowOff>323</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>819471</xdr:colOff>
+      <xdr:row>145</xdr:row>
+      <xdr:rowOff>179164</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7537100B-56C7-990D-39A9-A0EB64D5CC55}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="966428" y="36018430"/>
+          <a:ext cx="7772400" cy="4369841"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>354429</xdr:colOff>
+      <xdr:row>147</xdr:row>
+      <xdr:rowOff>27858</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>819793</xdr:colOff>
+      <xdr:row>170</xdr:row>
+      <xdr:rowOff>16199</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77B0AF74-744A-C8FD-833F-519AB1B34355}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="966750" y="40617965"/>
+          <a:ext cx="7772400" cy="4369841"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1327,16 +1621,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{820B8536-4987-4D23-A1DF-107BD88A4060}">
-  <dimension ref="A1:I115"/>
+  <dimension ref="B1:I108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F73" sqref="F73"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="5.5703125" customWidth="1"/>
-    <col min="3" max="5" width="37" customWidth="1"/>
+    <col min="3" max="3" width="37" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" customWidth="1"/>
+    <col min="5" max="5" width="37" customWidth="1"/>
     <col min="6" max="6" width="44.85546875" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
     <col min="8" max="8" width="19.42578125" customWidth="1"/>
@@ -1344,159 +1640,152 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="D1" s="56"/>
+      <c r="D1" s="27"/>
     </row>
     <row r="2" spans="2:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="D2" s="56" t="s">
+      <c r="D2" s="27" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="25">
+      <c r="C3" s="20">
         <v>211110476</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="23" t="s">
         <v>69</v>
       </c>
+      <c r="F3" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="4" spans="2:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="25">
+      <c r="C4" s="20">
         <v>211110404</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="20" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="25">
+      <c r="C5" s="20">
         <v>211110443</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="20" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="2:9" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+    </row>
     <row r="7" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="62"/>
+    </row>
+    <row r="8" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C8" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D8" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E8" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F8" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H8" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="11">
+    <row r="9" spans="2:9" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="11">
         <v>5</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C9" s="64" t="s">
         <v>88</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D9" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="E9" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="29" t="s">
+      <c r="F9" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G9" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="3">
-        <v>5</v>
-      </c>
-      <c r="I8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="12">
-        <v>6</v>
-      </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" s="4">
+      <c r="H9" s="3">
         <v>5</v>
       </c>
       <c r="I9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="12">
-        <v>8</v>
-      </c>
-      <c r="C10" s="36" t="s">
-        <v>89</v>
-      </c>
-      <c r="D10" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="31" t="s">
-        <v>37</v>
+      <c r="C10" s="65"/>
+      <c r="D10" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>34</v>
       </c>
       <c r="G10" s="14" t="s">
         <v>32</v>
       </c>
       <c r="H10" s="4">
+        <v>5</v>
+      </c>
+      <c r="I10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="12">
         <v>8</v>
       </c>
-      <c r="I10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="12">
-        <v>4</v>
-      </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="25" t="s">
+      <c r="C11" s="67" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="30" t="s">
+      <c r="E11" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="15" t="s">
-        <v>36</v>
+      <c r="G11" s="14" t="s">
+        <v>32</v>
       </c>
       <c r="H11" s="4">
         <v>8</v>
@@ -1505,45 +1794,45 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="12">
-        <v>11</v>
-      </c>
-      <c r="C12" s="27" t="s">
-        <v>90</v>
-      </c>
-      <c r="D12" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="65"/>
+      <c r="D12" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="30" t="s">
-        <v>43</v>
+      <c r="E12" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>37</v>
       </c>
       <c r="G12" s="15" t="s">
         <v>36</v>
       </c>
       <c r="H12" s="4">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I12" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="12">
-        <v>2</v>
-      </c>
-      <c r="C13" s="27"/>
-      <c r="D13" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="66" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="30" t="s">
-        <v>39</v>
+      <c r="E13" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>43</v>
       </c>
       <c r="G13" s="15" t="s">
         <v>36</v>
@@ -1555,1127 +1844,1090 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="2:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="12">
-        <v>3</v>
-      </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="66"/>
+      <c r="D14" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="30" t="s">
-        <v>40</v>
+      <c r="E14" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>39</v>
       </c>
       <c r="G14" s="15" t="s">
         <v>36</v>
       </c>
       <c r="H14" s="4">
+        <v>5</v>
+      </c>
+      <c r="I14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="12">
+        <v>3</v>
+      </c>
+      <c r="C15" s="66"/>
+      <c r="D15" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="I14" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="12">
-        <v>10</v>
-      </c>
-      <c r="C15" s="35"/>
-      <c r="D15" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="30" t="s">
-        <v>42</v>
+      <c r="F15" s="23" t="s">
+        <v>40</v>
       </c>
       <c r="G15" s="15" t="s">
         <v>36</v>
       </c>
       <c r="H15" s="4">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I15" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="12">
+        <v>10</v>
+      </c>
+      <c r="C16" s="65"/>
+      <c r="D16" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16" s="4">
+        <v>5</v>
+      </c>
+      <c r="I16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="12">
         <v>1</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C17" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="D16" s="25" t="s">
+      <c r="D17" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="30" t="s">
+      <c r="E17" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="30" t="s">
+      <c r="F17" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="G17" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H17" s="4">
         <v>13</v>
-      </c>
-      <c r="I16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="12">
-        <v>9</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="G17" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="H17" s="4">
-        <v>3</v>
       </c>
       <c r="I17" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="2:9" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="13">
+    <row r="18" spans="2:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="12">
+        <v>9</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="4">
+        <v>3</v>
+      </c>
+      <c r="I18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="13">
         <v>7</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C19" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="D18" s="25" t="s">
+      <c r="D19" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="33" t="s">
+      <c r="E19" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="34" t="s">
+      <c r="F19" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="G18" s="17" t="s">
+      <c r="G19" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="H18" s="5">
+      <c r="H19" s="5">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="20"/>
-      <c r="C21" s="21" t="s">
+    <row r="21" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="46"/>
+      <c r="C22" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="22"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C22" s="19" t="s">
+      <c r="D22" s="48"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="49"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="51"/>
+      <c r="C23" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18" t="s">
+      <c r="D23" s="40"/>
+      <c r="E23" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="F22" s="18" t="s">
+      <c r="F23" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+      <c r="G23" s="40"/>
+      <c r="H23" s="41"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24">
+      <c r="H24" s="42"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="52">
         <v>1</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25">
+      <c r="H25" s="42"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="52">
         <v>2</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+      <c r="H26" s="42"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27">
+      <c r="H27" s="42"/>
+    </row>
+    <row r="28" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="53">
         <v>1</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" s="44" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="18"/>
-      <c r="C29" s="18" t="s">
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="45"/>
+    </row>
+    <row r="29" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="38"/>
+      <c r="C30" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18" t="s">
+      <c r="D30" s="40"/>
+      <c r="E30" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="F29" s="18" t="s">
+      <c r="F30" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="18" t="s">
+      <c r="G30" s="40"/>
+      <c r="H30" s="41"/>
+    </row>
+    <row r="31" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C31" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31">
+      <c r="D31" s="48"/>
+      <c r="E31" s="48"/>
+      <c r="F31" s="48"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="49"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="52">
         <v>1</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32">
+      <c r="H32" s="42"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="52">
         <v>2</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B33">
+      <c r="H33" s="42"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="52">
         <v>3</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+      <c r="H34" s="42"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B35">
+      <c r="H35" s="42"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="52">
         <v>5</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B36">
+      <c r="H36" s="42"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="52">
         <v>6</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B37">
+      <c r="H37" s="42"/>
+    </row>
+    <row r="38" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="53">
         <v>9</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" s="44" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="18"/>
-      <c r="C39" s="18" t="s">
+      <c r="D38" s="44"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="44"/>
+      <c r="G38" s="44"/>
+      <c r="H38" s="45"/>
+    </row>
+    <row r="39" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="38"/>
+      <c r="C40" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18" t="s">
+      <c r="D40" s="40"/>
+      <c r="E40" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="18"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="18" t="s">
+      <c r="F40" s="40"/>
+      <c r="G40" s="40"/>
+      <c r="H40" s="41"/>
+    </row>
+    <row r="41" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="C40" s="18" t="s">
+      <c r="C41" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="20"/>
-      <c r="B41" s="20">
+      <c r="D41" s="48"/>
+      <c r="E41" s="48"/>
+      <c r="F41" s="48"/>
+      <c r="G41" s="48"/>
+      <c r="H41" s="49"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="52">
         <v>1</v>
       </c>
-      <c r="C41" s="39" t="s">
+      <c r="C42" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-    </row>
-    <row r="42" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="20"/>
-      <c r="B42" s="20">
+      <c r="H42" s="42"/>
+    </row>
+    <row r="43" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="52">
         <v>2</v>
       </c>
-      <c r="C42" s="39" t="s">
+      <c r="C43" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-    </row>
-    <row r="43" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="20"/>
-      <c r="B43" s="20">
+      <c r="H43" s="42"/>
+    </row>
+    <row r="44" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="52">
         <v>3</v>
       </c>
-      <c r="C43" s="39" t="s">
+      <c r="C44" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-    </row>
-    <row r="44" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="20"/>
-      <c r="B44" s="40">
+      <c r="H44" s="42"/>
+    </row>
+    <row r="45" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="52">
         <v>4</v>
       </c>
-      <c r="C44" s="39" t="s">
+      <c r="C45" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="20"/>
-      <c r="B45" s="20" t="s">
+      <c r="H45" s="42"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C45" s="20" t="s">
+      <c r="C46" t="s">
         <v>22</v>
       </c>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="20"/>
-      <c r="B46" s="38">
+      <c r="H46" s="42"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="54">
         <v>8</v>
       </c>
-      <c r="C46" s="39" t="s">
+      <c r="C47" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="D46" s="20"/>
-      <c r="E46" s="20"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="20"/>
-      <c r="B47" s="38">
+      <c r="H47" s="42"/>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B48" s="54">
         <v>4</v>
       </c>
-      <c r="C47" s="39" t="s">
+      <c r="C48" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="20"/>
-      <c r="B48" s="38">
+      <c r="H48" s="42"/>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49" s="54">
         <v>11</v>
       </c>
-      <c r="C48" s="39" t="s">
+      <c r="C49" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="D48" s="20"/>
-      <c r="E48" s="20"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="20"/>
-      <c r="B49" s="38">
+      <c r="H49" s="42"/>
+    </row>
+    <row r="50" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="55">
         <v>2</v>
       </c>
-      <c r="C49" s="39" t="s">
+      <c r="C50" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="D49" s="20"/>
-      <c r="E49" s="20"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="20"/>
-      <c r="B50" s="20"/>
-      <c r="C50" s="20" t="s">
+      <c r="D50" s="44"/>
+      <c r="E50" s="44"/>
+      <c r="F50" s="44"/>
+      <c r="G50" s="44"/>
+      <c r="H50" s="45"/>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B51" s="27"/>
+      <c r="C51" t="s">
         <v>28</v>
       </c>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C51" s="42" t="s">
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C53" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="D51" s="42"/>
-      <c r="E51" s="42"/>
-      <c r="F51" s="42"/>
-      <c r="G51" s="42"/>
-      <c r="H51" s="42"/>
-    </row>
-    <row r="52" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C52" s="2" t="s">
+      <c r="D53" s="29"/>
+      <c r="E53" s="29"/>
+      <c r="F53" s="29"/>
+      <c r="G53" s="29"/>
+      <c r="H53" s="29"/>
+    </row>
+    <row r="54" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C54" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="D54" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E52" s="2" t="s">
+      <c r="E54" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="F54" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G52" s="2" t="s">
+      <c r="G54" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H52" s="2" t="s">
+      <c r="H54" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C53" s="2">
+    <row r="55" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C55" s="2">
         <v>1</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="D55" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E53" s="2" t="s">
+      <c r="E55" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F53" s="51">
-        <v>45043</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="H53" s="51">
-        <v>45043</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C54" s="2">
-        <v>2</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F54" s="51">
-        <v>45043</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="H54" s="51">
-        <v>45043</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="C55" s="2">
-        <v>3</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F55" s="51">
+      <c r="F55" s="35">
         <v>45043</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H55" s="51">
+      <c r="H55" s="35">
         <v>45043</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C56" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F56" s="51">
-        <v>45044</v>
+        <v>74</v>
+      </c>
+      <c r="F56" s="35">
+        <v>45043</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H56" s="51">
-        <v>45044</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H56" s="35">
+        <v>45043</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="C57" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F57" s="51">
-        <v>45044</v>
+        <v>75</v>
+      </c>
+      <c r="F57" s="35">
+        <v>45043</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H57" s="51">
+      <c r="H57" s="35">
+        <v>45043</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C58" s="2">
+        <v>4</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F58" s="35">
         <v>45044</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C58" s="2">
-        <v>6</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F58" s="51">
-        <v>45045</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H58" s="51">
-        <v>45045</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H58" s="35">
+        <v>45044</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C59" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F59" s="51">
-        <v>45045</v>
+        <v>77</v>
+      </c>
+      <c r="F59" s="35">
+        <v>45044</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H59" s="51">
+      <c r="H59" s="35">
+        <v>45044</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C60" s="2">
+        <v>6</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F60" s="35">
         <v>45045</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C60" s="2">
-        <v>8</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="F60" s="51">
-        <v>45046</v>
       </c>
       <c r="G60" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H60" s="51">
-        <v>45046</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H60" s="35">
+        <v>45045</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C61" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F61" s="51">
-        <v>45046</v>
+        <v>80</v>
+      </c>
+      <c r="F61" s="35">
+        <v>45045</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H61" s="51">
-        <v>45046</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H61" s="35">
+        <v>45045</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C62" s="2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>69</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F62" s="51">
-        <v>45047</v>
+        <v>81</v>
+      </c>
+      <c r="F62" s="35">
+        <v>45046</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H62" s="51">
-        <v>45047</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H62" s="35">
+        <v>45046</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C63" s="2">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F63" s="51">
-        <v>45048</v>
+        <v>82</v>
+      </c>
+      <c r="F63" s="35">
+        <v>45046</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H63" s="51">
-        <v>45048</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H63" s="35">
+        <v>45046</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C64" s="2">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F64" s="51">
-        <v>45049</v>
+        <v>83</v>
+      </c>
+      <c r="F64" s="35">
+        <v>45047</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H64" s="51">
+      <c r="H64" s="35">
+        <v>45047</v>
+      </c>
+    </row>
+    <row r="65" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C65" s="2">
+        <v>11</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F65" s="35">
+        <v>45048</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H65" s="35">
+        <v>45048</v>
+      </c>
+    </row>
+    <row r="66" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C66" s="2">
+        <v>12</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F66" s="35">
         <v>45049</v>
       </c>
-    </row>
-    <row r="66" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C66" s="45" t="s">
+      <c r="G66" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H66" s="35">
+        <v>45049</v>
+      </c>
+    </row>
+    <row r="68" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C68" s="68" t="s">
         <v>55</v>
       </c>
-      <c r="D66" s="45"/>
-      <c r="E66" s="45"/>
-    </row>
-    <row r="67" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C67" s="46" t="s">
+      <c r="D68" s="68"/>
+      <c r="E68" s="68"/>
+    </row>
+    <row r="69" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C69" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="D67" s="46" t="s">
+      <c r="D69" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="E67" s="46" t="s">
+      <c r="E69" s="32" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="68" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C68" s="47" t="s">
+    <row r="70" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C70" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="D68" s="47"/>
-      <c r="E68" s="47"/>
-    </row>
-    <row r="69" spans="3:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="C69" s="43" t="s">
+      <c r="D70" s="59"/>
+      <c r="E70" s="59"/>
+    </row>
+    <row r="71" spans="3:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C71" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="D69" s="50" t="s">
+      <c r="D71" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="E69" s="43" t="s">
+      <c r="E71" s="30" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="70" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C70" s="47" t="s">
+    <row r="72" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C72" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="D70" s="47"/>
-      <c r="E70" s="47"/>
-    </row>
-    <row r="71" spans="3:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="C71" s="43" t="s">
+      <c r="D72" s="59"/>
+      <c r="E72" s="59"/>
+    </row>
+    <row r="73" spans="3:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C73" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D71" s="49" t="s">
+      <c r="D73" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="E71" s="43" t="s">
+      <c r="E73" s="30" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="72" spans="3:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="C72" s="43" t="s">
+    <row r="74" spans="3:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="C74" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="D72" s="49" t="s">
+      <c r="D74" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="E72" s="43"/>
-    </row>
-    <row r="73" spans="3:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="C73" s="43" t="s">
+      <c r="E74" s="30"/>
+    </row>
+    <row r="75" spans="3:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C75" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="D73" s="49" t="s">
+      <c r="D75" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="E73" s="43"/>
-    </row>
-    <row r="74" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C74" s="47" t="s">
+      <c r="E75" s="30"/>
+    </row>
+    <row r="76" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C76" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="D74" s="47"/>
-      <c r="E74" s="47"/>
-    </row>
-    <row r="75" spans="3:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="C75" s="43" t="s">
+      <c r="D76" s="59"/>
+      <c r="E76" s="59"/>
+    </row>
+    <row r="77" spans="3:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C77" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="D75" s="44" t="s">
+      <c r="D77" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E75" s="43" t="s">
+      <c r="E77" s="30" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="76" spans="3:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="C76" s="48"/>
-      <c r="D76" s="44" t="s">
+    <row r="78" spans="3:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="C78" s="33"/>
+      <c r="D78" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="E76" s="48"/>
-    </row>
-    <row r="77" spans="3:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="C77" s="48"/>
-      <c r="D77" s="44" t="s">
+      <c r="E78" s="33"/>
+    </row>
+    <row r="79" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C79" s="33"/>
+      <c r="D79" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="E77" s="48"/>
-    </row>
-    <row r="78" spans="3:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="C78" s="48"/>
-      <c r="D78" s="44" t="s">
+      <c r="E79" s="33"/>
+    </row>
+    <row r="80" spans="3:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C80" s="33"/>
+      <c r="D80" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="E78" s="48"/>
-    </row>
-    <row r="79" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C79" s="41"/>
-      <c r="D79" s="41"/>
-      <c r="E79" s="41"/>
-    </row>
-    <row r="80" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C80" s="41"/>
-      <c r="D80" s="41"/>
-      <c r="E80" s="41"/>
+      <c r="E80" s="33"/>
+    </row>
+    <row r="81" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C81" s="28"/>
+      <c r="D81" s="28"/>
+      <c r="E81" s="28"/>
     </row>
     <row r="82" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C82" s="52" t="s">
+      <c r="C82" s="28"/>
+      <c r="D82" s="28"/>
+      <c r="E82" s="28"/>
+    </row>
+    <row r="84" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C84" s="69" t="s">
         <v>59</v>
       </c>
-      <c r="D82" s="52"/>
-      <c r="E82" s="52"/>
-      <c r="F82" s="52"/>
-      <c r="G82" s="52"/>
-    </row>
-    <row r="83" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C83" s="53" t="s">
+      <c r="D84" s="69"/>
+      <c r="E84" s="69"/>
+      <c r="F84" s="69"/>
+      <c r="G84" s="69"/>
+    </row>
+    <row r="85" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C85" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="D83" s="53"/>
-      <c r="E83" s="53" t="s">
+      <c r="D85" s="63"/>
+      <c r="E85" s="63" t="s">
         <v>61</v>
       </c>
-      <c r="F83" s="53"/>
-      <c r="G83" s="53"/>
-    </row>
-    <row r="84" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C84" s="55" t="s">
+      <c r="F85" s="63"/>
+      <c r="G85" s="63"/>
+    </row>
+    <row r="86" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C86" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="D84" s="55" t="s">
+      <c r="D86" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="E84" s="55" t="s">
+      <c r="E86" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="F84" s="55" t="s">
+      <c r="F86" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="G84" s="55" t="s">
+      <c r="G86" s="36" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="85" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C85" s="54" t="s">
+    <row r="87" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C87" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="D85" s="54"/>
-      <c r="E85" s="54"/>
-      <c r="F85" s="54"/>
-      <c r="G85" s="54"/>
-    </row>
-    <row r="86" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C86" s="25" t="s">
+      <c r="D87" s="58"/>
+      <c r="E87" s="58"/>
+      <c r="F87" s="58"/>
+      <c r="G87" s="58"/>
+    </row>
+    <row r="88" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C88" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="D86" s="25" t="s">
+      <c r="D88" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="E86" s="25" t="s">
+      <c r="E88" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="F86" s="25" t="s">
+      <c r="F88" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="G86" s="25" t="s">
+      <c r="G88" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="87" spans="3:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="C87" s="25"/>
-      <c r="D87" s="25"/>
-      <c r="E87" s="25"/>
-      <c r="F87" s="25"/>
-      <c r="G87" s="30" t="s">
+    <row r="89" spans="3:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="C89" s="20"/>
+      <c r="D89" s="20"/>
+      <c r="E89" s="20"/>
+      <c r="F89" s="20"/>
+      <c r="G89" s="23" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="88" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C88" s="54" t="s">
+    <row r="90" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C90" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="D88" s="54"/>
-      <c r="E88" s="54"/>
-      <c r="F88" s="54"/>
-      <c r="G88" s="54"/>
-    </row>
-    <row r="89" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C89" s="25" t="s">
+      <c r="D90" s="58"/>
+      <c r="E90" s="58"/>
+      <c r="F90" s="58"/>
+      <c r="G90" s="58"/>
+    </row>
+    <row r="91" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C91" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="D89" s="25" t="s">
+      <c r="D91" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="E89" s="25" t="s">
+      <c r="E91" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="F89" s="25" t="s">
+      <c r="F91" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="G89" s="25" t="s">
+      <c r="G91" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="90" spans="3:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C90" s="30" t="s">
+    <row r="92" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C92" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="D90" s="25"/>
-      <c r="E90" s="25"/>
-      <c r="F90" s="30" t="s">
+      <c r="D92" s="20"/>
+      <c r="E92" s="20"/>
+      <c r="F92" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="G90" s="25"/>
-    </row>
-    <row r="91" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C91" s="54" t="s">
+      <c r="G92" s="20"/>
+    </row>
+    <row r="93" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C93" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D91" s="54"/>
-      <c r="E91" s="54"/>
-      <c r="F91" s="54"/>
-      <c r="G91" s="54"/>
-    </row>
-    <row r="92" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C92" s="25"/>
-      <c r="D92" s="25"/>
-      <c r="E92" s="25"/>
-      <c r="F92" s="25"/>
-      <c r="G92" s="25"/>
-    </row>
-    <row r="93" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C93" s="25"/>
-      <c r="D93" s="25"/>
-      <c r="E93" s="25"/>
-      <c r="F93" s="25"/>
-      <c r="G93" s="25"/>
+      <c r="D93" s="58"/>
+      <c r="E93" s="58"/>
+      <c r="F93" s="58"/>
+      <c r="G93" s="58"/>
     </row>
     <row r="94" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C94" s="25"/>
-      <c r="D94" s="25"/>
-      <c r="E94" s="25"/>
-      <c r="F94" s="25"/>
-      <c r="G94" s="25"/>
+      <c r="C94" s="20"/>
+      <c r="D94" s="20"/>
+      <c r="E94" s="20"/>
+      <c r="F94" s="20"/>
+      <c r="G94" s="20"/>
     </row>
     <row r="95" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C95" s="25"/>
-      <c r="D95" s="25"/>
-      <c r="E95" s="25"/>
-      <c r="F95" s="25"/>
-      <c r="G95" s="25"/>
+      <c r="C95" s="20"/>
+      <c r="D95" s="20"/>
+      <c r="E95" s="20"/>
+      <c r="F95" s="20"/>
+      <c r="G95" s="20"/>
     </row>
     <row r="96" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C96" s="25"/>
-      <c r="D96" s="25"/>
-      <c r="E96" s="25"/>
-      <c r="F96" s="25"/>
-      <c r="G96" s="25"/>
+      <c r="C96" s="20"/>
+      <c r="D96" s="20"/>
+      <c r="E96" s="20"/>
+      <c r="F96" s="20"/>
+      <c r="G96" s="20"/>
     </row>
     <row r="97" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C97" s="25"/>
-      <c r="D97" s="25"/>
-      <c r="E97" s="25"/>
-      <c r="F97" s="25"/>
-      <c r="G97" s="25"/>
+      <c r="C97" s="27"/>
+      <c r="D97" s="27"/>
+      <c r="E97" s="27"/>
+      <c r="F97" s="27"/>
+      <c r="G97" s="27"/>
     </row>
     <row r="98" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C98" s="25"/>
-      <c r="D98" s="25"/>
-      <c r="E98" s="25"/>
-      <c r="F98" s="25"/>
-      <c r="G98" s="25"/>
+      <c r="C98" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="D98" s="27"/>
+      <c r="E98" s="27"/>
+      <c r="F98" s="27"/>
+      <c r="G98" s="27"/>
     </row>
     <row r="99" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C99" s="25"/>
-      <c r="D99" s="25"/>
-      <c r="E99" s="25"/>
-      <c r="F99" s="25"/>
-      <c r="G99" s="25"/>
+      <c r="C99" s="27"/>
+      <c r="D99" s="27"/>
+      <c r="E99" s="27"/>
+      <c r="F99" s="27"/>
+      <c r="G99" s="27"/>
     </row>
     <row r="100" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C100" s="25"/>
-      <c r="D100" s="25"/>
-      <c r="E100" s="25"/>
-      <c r="F100" s="25"/>
-      <c r="G100" s="25"/>
+      <c r="C100" s="27"/>
+      <c r="D100" s="27"/>
+      <c r="E100" s="27"/>
+      <c r="F100" s="27"/>
+      <c r="G100" s="27"/>
     </row>
     <row r="101" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C101" s="25"/>
-      <c r="D101" s="25"/>
-      <c r="E101" s="25"/>
-      <c r="F101" s="25"/>
-      <c r="G101" s="25"/>
+      <c r="C101" s="27"/>
+      <c r="D101" s="27"/>
+      <c r="E101" s="27"/>
+      <c r="F101" s="27"/>
+      <c r="G101" s="27"/>
     </row>
     <row r="102" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C102" s="25"/>
-      <c r="D102" s="25"/>
-      <c r="E102" s="25"/>
-      <c r="F102" s="25"/>
-      <c r="G102" s="25"/>
+      <c r="C102" s="27"/>
+      <c r="D102" s="27"/>
+      <c r="E102" s="27"/>
+      <c r="F102" s="27"/>
+      <c r="G102" s="27"/>
     </row>
     <row r="103" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C103" s="25"/>
-      <c r="D103" s="25"/>
-      <c r="E103" s="25"/>
-      <c r="F103" s="25"/>
-      <c r="G103" s="25"/>
+      <c r="C103" s="27"/>
+      <c r="D103" s="27"/>
+      <c r="E103" s="27"/>
+      <c r="F103" s="27"/>
+      <c r="G103" s="27"/>
     </row>
     <row r="104" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C104" s="25"/>
-      <c r="D104" s="25"/>
-      <c r="E104" s="25"/>
-      <c r="F104" s="25"/>
-      <c r="G104" s="25"/>
+      <c r="C104" s="27"/>
+      <c r="D104" s="27"/>
+      <c r="E104" s="27"/>
+      <c r="F104" s="27"/>
+      <c r="G104" s="27"/>
     </row>
     <row r="105" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C105" s="25"/>
-      <c r="D105" s="25"/>
-      <c r="E105" s="25"/>
-      <c r="F105" s="25"/>
-      <c r="G105" s="25"/>
-    </row>
-    <row r="110" spans="3:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C110" s="52" t="s">
-        <v>59</v>
-      </c>
-      <c r="D110" s="52"/>
-      <c r="E110" s="52"/>
-      <c r="F110" s="52"/>
-      <c r="G110" s="52"/>
-    </row>
-    <row r="111" spans="3:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C111" s="53" t="s">
-        <v>60</v>
-      </c>
-      <c r="D111" s="53"/>
-      <c r="E111" s="53" t="s">
-        <v>61</v>
-      </c>
-      <c r="F111" s="53"/>
-      <c r="G111" s="53"/>
-    </row>
-    <row r="112" spans="3:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C112" s="55" t="s">
-        <v>62</v>
-      </c>
-      <c r="D112" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="E112" s="55" t="s">
-        <v>64</v>
-      </c>
-      <c r="F112" s="55" t="s">
-        <v>65</v>
-      </c>
-      <c r="G112" s="55" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="113" spans="3:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C113" s="54" t="s">
-        <v>26</v>
-      </c>
-      <c r="D113" s="54"/>
-      <c r="E113" s="54"/>
-      <c r="F113" s="54"/>
-      <c r="G113" s="54"/>
-    </row>
-    <row r="114" spans="3:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C114" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="D114" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="E114" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="F114" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="G114" s="25" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="115" spans="3:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C115" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="D115" s="25"/>
-      <c r="E115" s="25"/>
-      <c r="F115" s="30" t="s">
-        <v>106</v>
-      </c>
-      <c r="G115" s="25"/>
+      <c r="C105" s="27"/>
+      <c r="D105" s="27"/>
+      <c r="E105" s="27"/>
+      <c r="F105" s="27"/>
+      <c r="G105" s="27"/>
+    </row>
+    <row r="106" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C106" s="27"/>
+      <c r="D106" s="27"/>
+      <c r="E106" s="27"/>
+      <c r="F106" s="27"/>
+      <c r="G106" s="27"/>
+    </row>
+    <row r="107" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C107" s="27"/>
+      <c r="D107" s="27"/>
+      <c r="E107" s="27"/>
+      <c r="F107" s="27"/>
+      <c r="G107" s="27"/>
+    </row>
+    <row r="108" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C108" s="27"/>
+      <c r="D108" s="27"/>
+      <c r="E108" s="27"/>
+      <c r="F108" s="27"/>
+      <c r="G108" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="C111:D111"/>
-    <mergeCell ref="E111:G111"/>
-    <mergeCell ref="C113:G113"/>
-    <mergeCell ref="C110:G110"/>
-    <mergeCell ref="C88:G88"/>
-    <mergeCell ref="C91:G91"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="E83:G83"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="C10:C11"/>
+  <mergeCells count="14">
+    <mergeCell ref="C90:G90"/>
+    <mergeCell ref="C93:G93"/>
+    <mergeCell ref="C87:G87"/>
+    <mergeCell ref="C76:E76"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="E85:G85"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C68:E68"/>
     <mergeCell ref="C70:E70"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="C82:G82"/>
-    <mergeCell ref="C85:G85"/>
-    <mergeCell ref="C74:E74"/>
+    <mergeCell ref="C84:G84"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="8" scale="85" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
menambah back button dan laporan UTS (finish)
</commit_message>
<xml_diff>
--- a/Product Backlog+User Story.xlsx
+++ b/Product Backlog+User Story.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\version control git\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Music\sem4\3 agile\figma n laporan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5145200-554E-4AEE-A494-B6BEEB47CF8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7968E782-5D88-4086-8067-A843383A70B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2E39C133-9BD4-4088-A2A7-6E9E70B08AB9}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2E39C133-9BD4-4088-A2A7-6E9E70B08AB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="112">
   <si>
     <t>ID</t>
   </si>
@@ -318,9 +318,6 @@
     <t>Sistem Feedback</t>
   </si>
   <si>
-    <t>in-progress</t>
-  </si>
-  <si>
     <t>product backlog</t>
   </si>
   <si>
@@ -370,6 +367,9 @@
   </si>
   <si>
     <t>Screenshot board trello</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -455,7 +455,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -515,7 +515,7 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -527,55 +527,10 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -895,6 +850,58 @@
       </right>
       <top/>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -904,7 +911,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -915,34 +922,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -954,34 +952,28 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1015,77 +1007,101 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1170,7 +1186,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>832756</xdr:colOff>
+      <xdr:colOff>2030184</xdr:colOff>
       <xdr:row>121</xdr:row>
       <xdr:rowOff>15555</xdr:rowOff>
     </xdr:to>
@@ -1220,7 +1236,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>819471</xdr:colOff>
+      <xdr:colOff>2016899</xdr:colOff>
       <xdr:row>145</xdr:row>
       <xdr:rowOff>179164</xdr:rowOff>
     </xdr:to>
@@ -1270,7 +1286,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>819793</xdr:colOff>
+      <xdr:colOff>2017221</xdr:colOff>
       <xdr:row>170</xdr:row>
       <xdr:rowOff>16199</xdr:rowOff>
     </xdr:to>
@@ -1624,13 +1640,13 @@
   <dimension ref="B1:I108"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="5.5703125" customWidth="1"/>
-    <col min="3" max="3" width="37" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="30.28515625" customWidth="1"/>
     <col min="5" max="5" width="37" customWidth="1"/>
     <col min="6" max="6" width="44.85546875" customWidth="1"/>
@@ -1640,355 +1656,362 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="22"/>
+    </row>
+    <row r="2" spans="2:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="D1" s="27"/>
-    </row>
-    <row r="2" spans="2:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="27" t="s">
+      <c r="D2" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="D2" s="27" t="s">
-        <v>104</v>
-      </c>
     </row>
     <row r="3" spans="2:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="20">
+      <c r="C3" s="15">
         <v>211110476</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="18" t="s">
         <v>69</v>
       </c>
       <c r="F3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="20">
+      <c r="C4" s="15">
         <v>211110404</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="15" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="20">
+      <c r="C5" s="15">
         <v>211110443</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="15" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
     </row>
     <row r="7" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="61"/>
+      <c r="B7" s="61" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
       <c r="H7" s="62"/>
+      <c r="I7" s="63"/>
     </row>
     <row r="8" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="57" t="s">
         <v>4</v>
       </c>
+      <c r="I8" s="66" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="9" spans="2:9" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="11">
+      <c r="B9" s="8">
         <v>5</v>
       </c>
-      <c r="C9" s="64" t="s">
+      <c r="C9" s="67" t="s">
         <v>88</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="22" t="s">
+      <c r="F9" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="58">
         <v>5</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="65" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="12">
+      <c r="B10" s="9">
         <v>6</v>
       </c>
-      <c r="C10" s="65"/>
-      <c r="D10" s="20" t="s">
+      <c r="C10" s="68"/>
+      <c r="D10" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="23" t="s">
+      <c r="E10" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="F10" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="59">
         <v>5</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="12">
+      <c r="B11" s="9">
         <v>8</v>
       </c>
-      <c r="C11" s="67" t="s">
+      <c r="C11" s="69" t="s">
         <v>89</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="56" t="s">
+      <c r="F11" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="59">
         <v>8</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="9">
+        <v>4</v>
+      </c>
+      <c r="C12" s="68"/>
+      <c r="D12" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" s="59">
+        <v>8</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="9">
+        <v>11</v>
+      </c>
+      <c r="C13" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="59">
+        <v>5</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="9">
+        <v>2</v>
+      </c>
+      <c r="C14" s="70"/>
+      <c r="D14" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" s="59">
+        <v>5</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="9">
+        <v>3</v>
+      </c>
+      <c r="C15" s="70"/>
+      <c r="D15" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H15" s="59">
+        <v>8</v>
+      </c>
+      <c r="I15" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="12">
-        <v>4</v>
-      </c>
-      <c r="C12" s="65"/>
-      <c r="D12" s="20" t="s">
+    <row r="16" spans="2:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="9">
+        <v>10</v>
+      </c>
+      <c r="C16" s="68"/>
+      <c r="D16" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="23" t="s">
+      <c r="E16" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16" s="59">
+        <v>5</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="9">
+        <v>1</v>
+      </c>
+      <c r="C17" s="71" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="59">
+        <v>13</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="9">
         <v>9</v>
       </c>
-      <c r="F12" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="H12" s="4">
-        <v>8</v>
-      </c>
-      <c r="I12" t="s">
+      <c r="C18" s="71" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="59">
+        <v>3</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="10">
+        <v>7</v>
+      </c>
+      <c r="C19" s="72" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="H19" s="60">
+        <v>21</v>
+      </c>
+      <c r="I19" s="3" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="12">
-        <v>11</v>
-      </c>
-      <c r="C13" s="66" t="s">
-        <v>90</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="H13" s="4">
-        <v>5</v>
-      </c>
-      <c r="I13" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="12">
-        <v>2</v>
-      </c>
-      <c r="C14" s="66"/>
-      <c r="D14" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="H14" s="4">
-        <v>5</v>
-      </c>
-      <c r="I14" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="12">
-        <v>3</v>
-      </c>
-      <c r="C15" s="66"/>
-      <c r="D15" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="H15" s="4">
-        <v>8</v>
-      </c>
-      <c r="I15" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="12">
-        <v>10</v>
-      </c>
-      <c r="C16" s="65"/>
-      <c r="D16" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="G16" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="H16" s="4">
-        <v>5</v>
-      </c>
-      <c r="I16" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="12">
-        <v>1</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="G17" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" s="4">
-        <v>13</v>
-      </c>
-      <c r="I17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="12">
-        <v>9</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="G18" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="H18" s="4">
-        <v>3</v>
-      </c>
-      <c r="I18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="13">
-        <v>7</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="D19" s="57" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="G19" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="H19" s="5">
-        <v>21</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -2002,303 +2025,303 @@
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="46"/>
-      <c r="C22" s="47" t="s">
+      <c r="B22" s="41"/>
+      <c r="C22" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="48"/>
-      <c r="E22" s="48"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="48"/>
-      <c r="H22" s="49"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="44"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="51"/>
-      <c r="C23" s="39" t="s">
+      <c r="B23" s="46"/>
+      <c r="C23" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40" t="s">
+      <c r="D23" s="35"/>
+      <c r="E23" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="F23" s="40" t="s">
+      <c r="F23" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="G23" s="40"/>
-      <c r="H23" s="41"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="36"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="52" t="s">
+      <c r="B24" s="47" t="s">
         <v>25</v>
       </c>
       <c r="C24" t="s">
         <v>21</v>
       </c>
-      <c r="H24" s="42"/>
+      <c r="H24" s="37"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="52">
+      <c r="B25" s="47">
         <v>1</v>
       </c>
       <c r="C25" t="s">
         <v>23</v>
       </c>
-      <c r="H25" s="42"/>
+      <c r="H25" s="37"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="52">
+      <c r="B26" s="47">
         <v>2</v>
       </c>
       <c r="C26" t="s">
         <v>24</v>
       </c>
-      <c r="H26" s="42"/>
+      <c r="H26" s="37"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="52" t="s">
+      <c r="B27" s="47" t="s">
         <v>0</v>
       </c>
       <c r="C27" t="s">
         <v>22</v>
       </c>
-      <c r="H27" s="42"/>
+      <c r="H27" s="37"/>
     </row>
     <row r="28" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="53">
+      <c r="B28" s="48">
         <v>1</v>
       </c>
-      <c r="C28" s="44" t="s">
+      <c r="C28" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="44"/>
-      <c r="E28" s="44"/>
-      <c r="F28" s="44"/>
-      <c r="G28" s="44"/>
-      <c r="H28" s="45"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="40"/>
     </row>
     <row r="29" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="38"/>
-      <c r="C30" s="40" t="s">
+      <c r="B30" s="33"/>
+      <c r="C30" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40" t="s">
+      <c r="D30" s="35"/>
+      <c r="E30" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="F30" s="40" t="s">
+      <c r="F30" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="G30" s="40"/>
-      <c r="H30" s="41"/>
+      <c r="G30" s="35"/>
+      <c r="H30" s="36"/>
     </row>
     <row r="31" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="51" t="s">
+      <c r="B31" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="46" t="s">
+      <c r="C31" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="D31" s="48"/>
-      <c r="E31" s="48"/>
-      <c r="F31" s="48"/>
-      <c r="G31" s="48"/>
-      <c r="H31" s="49"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="44"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="52">
+      <c r="B32" s="47">
         <v>1</v>
       </c>
       <c r="C32" t="s">
         <v>33</v>
       </c>
-      <c r="H32" s="42"/>
+      <c r="H32" s="37"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="52">
+      <c r="B33" s="47">
         <v>2</v>
       </c>
       <c r="C33" t="s">
         <v>34</v>
       </c>
-      <c r="H33" s="42"/>
+      <c r="H33" s="37"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="52">
+      <c r="B34" s="47">
         <v>3</v>
       </c>
       <c r="C34" t="s">
         <v>41</v>
       </c>
-      <c r="H34" s="42"/>
+      <c r="H34" s="37"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="52" t="s">
+      <c r="B35" s="47" t="s">
         <v>0</v>
       </c>
       <c r="C35" t="s">
         <v>22</v>
       </c>
-      <c r="H35" s="42"/>
+      <c r="H35" s="37"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="52">
+      <c r="B36" s="47">
         <v>5</v>
       </c>
       <c r="C36" t="s">
         <v>10</v>
       </c>
-      <c r="H36" s="42"/>
+      <c r="H36" s="37"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="52">
+      <c r="B37" s="47">
         <v>6</v>
       </c>
       <c r="C37" t="s">
         <v>15</v>
       </c>
-      <c r="H37" s="42"/>
+      <c r="H37" s="37"/>
     </row>
     <row r="38" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="53">
+      <c r="B38" s="48">
         <v>9</v>
       </c>
-      <c r="C38" s="44" t="s">
+      <c r="C38" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="D38" s="44"/>
-      <c r="E38" s="44"/>
-      <c r="F38" s="44"/>
-      <c r="G38" s="44"/>
-      <c r="H38" s="45"/>
+      <c r="D38" s="39"/>
+      <c r="E38" s="39"/>
+      <c r="F38" s="39"/>
+      <c r="G38" s="39"/>
+      <c r="H38" s="40"/>
     </row>
     <row r="39" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="40" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="38"/>
-      <c r="C40" s="40" t="s">
+      <c r="B40" s="33"/>
+      <c r="C40" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="D40" s="40"/>
-      <c r="E40" s="40" t="s">
-        <v>108</v>
-      </c>
-      <c r="F40" s="40"/>
-      <c r="G40" s="40"/>
-      <c r="H40" s="41"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="F40" s="35"/>
+      <c r="G40" s="35"/>
+      <c r="H40" s="36"/>
     </row>
     <row r="41" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="51" t="s">
+      <c r="B41" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C41" s="46" t="s">
+      <c r="C41" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="D41" s="48"/>
-      <c r="E41" s="48"/>
-      <c r="F41" s="48"/>
-      <c r="G41" s="48"/>
-      <c r="H41" s="49"/>
+      <c r="D41" s="43"/>
+      <c r="E41" s="43"/>
+      <c r="F41" s="43"/>
+      <c r="G41" s="43"/>
+      <c r="H41" s="44"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="52">
+      <c r="B42" s="47">
         <v>1</v>
       </c>
-      <c r="C42" s="43" t="s">
+      <c r="C42" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="H42" s="42"/>
+      <c r="H42" s="37"/>
     </row>
     <row r="43" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="52">
+      <c r="B43" s="47">
         <v>2</v>
       </c>
-      <c r="C43" s="43" t="s">
+      <c r="C43" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="H43" s="42"/>
+      <c r="H43" s="37"/>
     </row>
     <row r="44" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="52">
+      <c r="B44" s="47">
         <v>3</v>
       </c>
-      <c r="C44" s="43" t="s">
+      <c r="C44" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="H44" s="42"/>
+      <c r="H44" s="37"/>
     </row>
     <row r="45" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="52">
+      <c r="B45" s="47">
         <v>4</v>
       </c>
-      <c r="C45" s="43" t="s">
+      <c r="C45" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="H45" s="42"/>
+      <c r="H45" s="37"/>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="52" t="s">
+      <c r="B46" s="47" t="s">
         <v>0</v>
       </c>
       <c r="C46" t="s">
         <v>22</v>
       </c>
-      <c r="H46" s="42"/>
+      <c r="H46" s="37"/>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="54">
+      <c r="B47" s="49">
         <v>8</v>
       </c>
-      <c r="C47" s="43" t="s">
+      <c r="C47" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="H47" s="42"/>
+      <c r="H47" s="37"/>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B48" s="54">
+      <c r="B48" s="49">
         <v>4</v>
       </c>
-      <c r="C48" s="43" t="s">
+      <c r="C48" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="H48" s="42"/>
+      <c r="H48" s="37"/>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B49" s="54">
+      <c r="B49" s="49">
         <v>11</v>
       </c>
-      <c r="C49" s="43" t="s">
+      <c r="C49" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="H49" s="42"/>
+      <c r="H49" s="37"/>
     </row>
     <row r="50" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="55">
+      <c r="B50" s="50">
         <v>2</v>
       </c>
-      <c r="C50" s="50" t="s">
+      <c r="C50" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D50" s="44"/>
-      <c r="E50" s="44"/>
-      <c r="F50" s="44"/>
-      <c r="G50" s="44"/>
-      <c r="H50" s="45"/>
+      <c r="D50" s="39"/>
+      <c r="E50" s="39"/>
+      <c r="F50" s="39"/>
+      <c r="G50" s="39"/>
+      <c r="H50" s="40"/>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B51" s="27"/>
+      <c r="B51" s="22"/>
       <c r="C51" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C53" s="29" t="s">
+      <c r="C53" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="D53" s="29"/>
-      <c r="E53" s="29"/>
-      <c r="F53" s="29"/>
-      <c r="G53" s="29"/>
-      <c r="H53" s="29"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="24"/>
+      <c r="F53" s="24"/>
+      <c r="G53" s="24"/>
+      <c r="H53" s="24"/>
     </row>
     <row r="54" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C54" s="2" t="s">
@@ -2330,13 +2353,13 @@
       <c r="E55" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F55" s="35">
+      <c r="F55" s="30">
         <v>45043</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H55" s="35">
+      <c r="H55" s="30">
         <v>45043</v>
       </c>
     </row>
@@ -2350,13 +2373,13 @@
       <c r="E56" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F56" s="35">
+      <c r="F56" s="30">
         <v>45043</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H56" s="35">
+      <c r="H56" s="30">
         <v>45043</v>
       </c>
     </row>
@@ -2370,13 +2393,13 @@
       <c r="E57" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F57" s="35">
+      <c r="F57" s="30">
         <v>45043</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H57" s="35">
+      <c r="H57" s="30">
         <v>45043</v>
       </c>
     </row>
@@ -2390,13 +2413,13 @@
       <c r="E58" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F58" s="35">
+      <c r="F58" s="30">
         <v>45044</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H58" s="35">
+      <c r="H58" s="30">
         <v>45044</v>
       </c>
     </row>
@@ -2410,13 +2433,13 @@
       <c r="E59" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F59" s="35">
+      <c r="F59" s="30">
         <v>45044</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H59" s="35">
+      <c r="H59" s="30">
         <v>45044</v>
       </c>
     </row>
@@ -2430,13 +2453,13 @@
       <c r="E60" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F60" s="35">
+      <c r="F60" s="30">
         <v>45045</v>
       </c>
       <c r="G60" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H60" s="35">
+      <c r="H60" s="30">
         <v>45045</v>
       </c>
     </row>
@@ -2450,13 +2473,13 @@
       <c r="E61" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F61" s="35">
+      <c r="F61" s="30">
         <v>45045</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H61" s="35">
+      <c r="H61" s="30">
         <v>45045</v>
       </c>
     </row>
@@ -2470,13 +2493,13 @@
       <c r="E62" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F62" s="35">
+      <c r="F62" s="30">
         <v>45046</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H62" s="35">
+      <c r="H62" s="30">
         <v>45046</v>
       </c>
     </row>
@@ -2490,13 +2513,13 @@
       <c r="E63" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F63" s="35">
+      <c r="F63" s="30">
         <v>45046</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H63" s="35">
+      <c r="H63" s="30">
         <v>45046</v>
       </c>
     </row>
@@ -2510,13 +2533,13 @@
       <c r="E64" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F64" s="35">
+      <c r="F64" s="30">
         <v>45047</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H64" s="35">
+      <c r="H64" s="30">
         <v>45047</v>
       </c>
     </row>
@@ -2530,13 +2553,13 @@
       <c r="E65" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F65" s="35">
+      <c r="F65" s="30">
         <v>45048</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H65" s="35">
+      <c r="H65" s="30">
         <v>45048</v>
       </c>
     </row>
@@ -2550,361 +2573,361 @@
       <c r="E66" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F66" s="35">
+      <c r="F66" s="30">
         <v>45049</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H66" s="35">
+      <c r="H66" s="30">
         <v>45049</v>
       </c>
     </row>
     <row r="68" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C68" s="68" t="s">
+      <c r="C68" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="D68" s="68"/>
-      <c r="E68" s="68"/>
+      <c r="D68" s="55"/>
+      <c r="E68" s="55"/>
     </row>
     <row r="69" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C69" s="32" t="s">
+      <c r="C69" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="D69" s="32" t="s">
+      <c r="D69" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="E69" s="32" t="s">
+      <c r="E69" s="27" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="70" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C70" s="59" t="s">
+      <c r="C70" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="D70" s="59"/>
-      <c r="E70" s="59"/>
+      <c r="D70" s="53"/>
+      <c r="E70" s="53"/>
     </row>
     <row r="71" spans="3:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="C71" s="30" t="s">
+      <c r="C71" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D71" s="34" t="s">
+      <c r="D71" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="E71" s="30" t="s">
+      <c r="E71" s="25" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="72" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C72" s="59" t="s">
+      <c r="C72" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="D72" s="59"/>
-      <c r="E72" s="59"/>
+      <c r="D72" s="53"/>
+      <c r="E72" s="53"/>
     </row>
     <row r="73" spans="3:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="C73" s="30" t="s">
+      <c r="C73" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D73" s="34" t="s">
+      <c r="D73" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="E73" s="30" t="s">
+      <c r="E73" s="25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="74" spans="3:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="C74" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D74" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="E74" s="25"/>
+    </row>
+    <row r="75" spans="3:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C75" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D75" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="E75" s="25"/>
+    </row>
+    <row r="76" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C76" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="D76" s="53"/>
+      <c r="E76" s="53"/>
+    </row>
+    <row r="77" spans="3:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C77" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D77" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E77" s="25" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="74" spans="3:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="C74" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="D74" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="E74" s="30"/>
-    </row>
-    <row r="75" spans="3:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="C75" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="D75" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="E75" s="30"/>
-    </row>
-    <row r="76" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C76" s="59" t="s">
+    <row r="78" spans="3:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C78" s="28"/>
+      <c r="D78" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E78" s="28"/>
+    </row>
+    <row r="79" spans="3:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C79" s="28"/>
+      <c r="D79" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E79" s="28"/>
+    </row>
+    <row r="80" spans="3:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C80" s="28"/>
+      <c r="D80" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E80" s="28"/>
+    </row>
+    <row r="81" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C81" s="23"/>
+      <c r="D81" s="23"/>
+      <c r="E81" s="23"/>
+    </row>
+    <row r="82" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C82" s="23"/>
+      <c r="D82" s="23"/>
+      <c r="E82" s="23"/>
+    </row>
+    <row r="84" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C84" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="D84" s="56"/>
+      <c r="E84" s="56"/>
+      <c r="F84" s="56"/>
+      <c r="G84" s="56"/>
+    </row>
+    <row r="85" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C85" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="D85" s="54"/>
+      <c r="E85" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="F85" s="54"/>
+      <c r="G85" s="54"/>
+    </row>
+    <row r="86" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C86" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="D86" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="E86" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="F86" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="G86" s="31" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="87" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C87" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="D87" s="52"/>
+      <c r="E87" s="52"/>
+      <c r="F87" s="52"/>
+      <c r="G87" s="52"/>
+    </row>
+    <row r="88" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C88" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D88" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="E88" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F88" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="G88" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="89" spans="3:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="C89" s="15"/>
+      <c r="D89" s="15"/>
+      <c r="E89" s="15"/>
+      <c r="F89" s="15"/>
+      <c r="G89" s="18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="90" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C90" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="D90" s="52"/>
+      <c r="E90" s="52"/>
+      <c r="F90" s="52"/>
+      <c r="G90" s="52"/>
+    </row>
+    <row r="91" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C91" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D91" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="E91" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="F91" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="G91" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="92" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C92" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D92" s="15"/>
+      <c r="E92" s="15"/>
+      <c r="F92" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="G92" s="15"/>
+    </row>
+    <row r="93" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C93" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="D76" s="59"/>
-      <c r="E76" s="59"/>
-    </row>
-    <row r="77" spans="3:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="C77" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="D77" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E77" s="30" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="78" spans="3:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="C78" s="33"/>
-      <c r="D78" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="E78" s="33"/>
-    </row>
-    <row r="79" spans="3:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C79" s="33"/>
-      <c r="D79" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="E79" s="33"/>
-    </row>
-    <row r="80" spans="3:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="C80" s="33"/>
-      <c r="D80" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="E80" s="33"/>
-    </row>
-    <row r="81" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C81" s="28"/>
-      <c r="D81" s="28"/>
-      <c r="E81" s="28"/>
-    </row>
-    <row r="82" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C82" s="28"/>
-      <c r="D82" s="28"/>
-      <c r="E82" s="28"/>
-    </row>
-    <row r="84" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C84" s="69" t="s">
-        <v>59</v>
-      </c>
-      <c r="D84" s="69"/>
-      <c r="E84" s="69"/>
-      <c r="F84" s="69"/>
-      <c r="G84" s="69"/>
-    </row>
-    <row r="85" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C85" s="63" t="s">
-        <v>60</v>
-      </c>
-      <c r="D85" s="63"/>
-      <c r="E85" s="63" t="s">
-        <v>61</v>
-      </c>
-      <c r="F85" s="63"/>
-      <c r="G85" s="63"/>
-    </row>
-    <row r="86" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C86" s="36" t="s">
-        <v>62</v>
-      </c>
-      <c r="D86" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="E86" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="F86" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="G86" s="36" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="87" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C87" s="58" t="s">
-        <v>20</v>
-      </c>
-      <c r="D87" s="58"/>
-      <c r="E87" s="58"/>
-      <c r="F87" s="58"/>
-      <c r="G87" s="58"/>
-    </row>
-    <row r="88" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C88" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="D88" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="E88" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="F88" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="G88" s="20" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="89" spans="3:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="C89" s="20"/>
-      <c r="D89" s="20"/>
-      <c r="E89" s="20"/>
-      <c r="F89" s="20"/>
-      <c r="G89" s="23" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="90" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C90" s="58" t="s">
-        <v>26</v>
-      </c>
-      <c r="D90" s="58"/>
-      <c r="E90" s="58"/>
-      <c r="F90" s="58"/>
-      <c r="G90" s="58"/>
-    </row>
-    <row r="91" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C91" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="D91" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="E91" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="F91" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="G91" s="20" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="92" spans="3:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C92" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="D92" s="20"/>
-      <c r="E92" s="20"/>
-      <c r="F92" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="G92" s="20"/>
-    </row>
-    <row r="93" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C93" s="58" t="s">
-        <v>30</v>
-      </c>
-      <c r="D93" s="58"/>
-      <c r="E93" s="58"/>
-      <c r="F93" s="58"/>
-      <c r="G93" s="58"/>
+      <c r="D93" s="52"/>
+      <c r="E93" s="52"/>
+      <c r="F93" s="52"/>
+      <c r="G93" s="52"/>
     </row>
     <row r="94" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C94" s="20"/>
-      <c r="D94" s="20"/>
-      <c r="E94" s="20"/>
-      <c r="F94" s="20"/>
-      <c r="G94" s="20"/>
+      <c r="C94" s="15"/>
+      <c r="D94" s="15"/>
+      <c r="E94" s="15"/>
+      <c r="F94" s="15"/>
+      <c r="G94" s="15"/>
     </row>
     <row r="95" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C95" s="20"/>
-      <c r="D95" s="20"/>
-      <c r="E95" s="20"/>
-      <c r="F95" s="20"/>
-      <c r="G95" s="20"/>
+      <c r="C95" s="15"/>
+      <c r="D95" s="15"/>
+      <c r="E95" s="15"/>
+      <c r="F95" s="15"/>
+      <c r="G95" s="15"/>
     </row>
     <row r="96" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C96" s="20"/>
-      <c r="D96" s="20"/>
-      <c r="E96" s="20"/>
-      <c r="F96" s="20"/>
-      <c r="G96" s="20"/>
+      <c r="C96" s="15"/>
+      <c r="D96" s="15"/>
+      <c r="E96" s="15"/>
+      <c r="F96" s="15"/>
+      <c r="G96" s="15"/>
     </row>
     <row r="97" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C97" s="27"/>
-      <c r="D97" s="27"/>
-      <c r="E97" s="27"/>
-      <c r="F97" s="27"/>
-      <c r="G97" s="27"/>
+      <c r="C97" s="22"/>
+      <c r="D97" s="22"/>
+      <c r="E97" s="22"/>
+      <c r="F97" s="22"/>
+      <c r="G97" s="22"/>
     </row>
     <row r="98" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C98" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="D98" s="27"/>
-      <c r="E98" s="27"/>
-      <c r="F98" s="27"/>
-      <c r="G98" s="27"/>
+      <c r="C98" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="D98" s="22"/>
+      <c r="E98" s="22"/>
+      <c r="F98" s="22"/>
+      <c r="G98" s="22"/>
     </row>
     <row r="99" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C99" s="27"/>
-      <c r="D99" s="27"/>
-      <c r="E99" s="27"/>
-      <c r="F99" s="27"/>
-      <c r="G99" s="27"/>
+      <c r="C99" s="22"/>
+      <c r="D99" s="22"/>
+      <c r="E99" s="22"/>
+      <c r="F99" s="22"/>
+      <c r="G99" s="22"/>
     </row>
     <row r="100" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C100" s="27"/>
-      <c r="D100" s="27"/>
-      <c r="E100" s="27"/>
-      <c r="F100" s="27"/>
-      <c r="G100" s="27"/>
+      <c r="C100" s="22"/>
+      <c r="D100" s="22"/>
+      <c r="E100" s="22"/>
+      <c r="F100" s="22"/>
+      <c r="G100" s="22"/>
     </row>
     <row r="101" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C101" s="27"/>
-      <c r="D101" s="27"/>
-      <c r="E101" s="27"/>
-      <c r="F101" s="27"/>
-      <c r="G101" s="27"/>
+      <c r="C101" s="22"/>
+      <c r="D101" s="22"/>
+      <c r="E101" s="22"/>
+      <c r="F101" s="22"/>
+      <c r="G101" s="22"/>
     </row>
     <row r="102" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C102" s="27"/>
-      <c r="D102" s="27"/>
-      <c r="E102" s="27"/>
-      <c r="F102" s="27"/>
-      <c r="G102" s="27"/>
+      <c r="C102" s="22"/>
+      <c r="D102" s="22"/>
+      <c r="E102" s="22"/>
+      <c r="F102" s="22"/>
+      <c r="G102" s="22"/>
     </row>
     <row r="103" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C103" s="27"/>
-      <c r="D103" s="27"/>
-      <c r="E103" s="27"/>
-      <c r="F103" s="27"/>
-      <c r="G103" s="27"/>
+      <c r="C103" s="22"/>
+      <c r="D103" s="22"/>
+      <c r="E103" s="22"/>
+      <c r="F103" s="22"/>
+      <c r="G103" s="22"/>
     </row>
     <row r="104" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C104" s="27"/>
-      <c r="D104" s="27"/>
-      <c r="E104" s="27"/>
-      <c r="F104" s="27"/>
-      <c r="G104" s="27"/>
+      <c r="C104" s="22"/>
+      <c r="D104" s="22"/>
+      <c r="E104" s="22"/>
+      <c r="F104" s="22"/>
+      <c r="G104" s="22"/>
     </row>
     <row r="105" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C105" s="27"/>
-      <c r="D105" s="27"/>
-      <c r="E105" s="27"/>
-      <c r="F105" s="27"/>
-      <c r="G105" s="27"/>
+      <c r="C105" s="22"/>
+      <c r="D105" s="22"/>
+      <c r="E105" s="22"/>
+      <c r="F105" s="22"/>
+      <c r="G105" s="22"/>
     </row>
     <row r="106" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C106" s="27"/>
-      <c r="D106" s="27"/>
-      <c r="E106" s="27"/>
-      <c r="F106" s="27"/>
-      <c r="G106" s="27"/>
+      <c r="C106" s="22"/>
+      <c r="D106" s="22"/>
+      <c r="E106" s="22"/>
+      <c r="F106" s="22"/>
+      <c r="G106" s="22"/>
     </row>
     <row r="107" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C107" s="27"/>
-      <c r="D107" s="27"/>
-      <c r="E107" s="27"/>
-      <c r="F107" s="27"/>
-      <c r="G107" s="27"/>
+      <c r="C107" s="22"/>
+      <c r="D107" s="22"/>
+      <c r="E107" s="22"/>
+      <c r="F107" s="22"/>
+      <c r="G107" s="22"/>
     </row>
     <row r="108" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C108" s="27"/>
-      <c r="D108" s="27"/>
-      <c r="E108" s="27"/>
-      <c r="F108" s="27"/>
-      <c r="G108" s="27"/>
+      <c r="C108" s="22"/>
+      <c r="D108" s="22"/>
+      <c r="E108" s="22"/>
+      <c r="F108" s="22"/>
+      <c r="G108" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -2912,7 +2935,6 @@
     <mergeCell ref="C93:G93"/>
     <mergeCell ref="C87:G87"/>
     <mergeCell ref="C76:E76"/>
-    <mergeCell ref="B7:H7"/>
     <mergeCell ref="C85:D85"/>
     <mergeCell ref="E85:G85"/>
     <mergeCell ref="C9:C10"/>
@@ -2922,6 +2944,7 @@
     <mergeCell ref="C68:E68"/>
     <mergeCell ref="C70:E70"/>
     <mergeCell ref="C84:G84"/>
+    <mergeCell ref="B7:I7"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" scale="85" orientation="landscape" r:id="rId1"/>

</xml_diff>